<commit_message>
add two columns & modify matching func
</commit_message>
<xml_diff>
--- a/data/2d_test2_matched.xlsx
+++ b/data/2d_test2_matched.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -38,7 +38,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFBB00"/>
+        <fgColor rgb="00FFC0CB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DC143C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFD700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFDEAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -61,12 +86,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -432,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +493,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Publisher</t>
+          <t>JOURNAL</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -479,6 +509,26 @@
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Reference_Count</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Affiliation1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Affiliation2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>RP</t>
         </is>
       </c>
     </row>
@@ -486,7 +536,7 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Zhang, Changsheng</t>
         </is>
@@ -508,12 +558,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ELSEVIER SCIENCE BV</t>
+          <t>JOURNAL OF MAGNETISM AND MAGNETIC MATERIALS</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -521,13 +571,23 @@
       </c>
       <c r="I2" t="n">
         <v>36</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Zhang, CS (reprint author), Inst Nucl Phys &amp; Chem, Key Lab Neutron Phys CAEP, Mianyang 621999, Sichuan, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Inst Nucl Phys &amp; Chem</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Ray, S. J.</t>
         </is>
@@ -549,12 +609,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>India</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -562,13 +622,23 @@
       </c>
       <c r="I3" t="n">
         <v>32</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Ray, SJ (reprint author), Indian Inst Technol Patna, Dept Phys, Bihta 801106, India.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Indian Inst Technol Patna</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Zhang, Zhenyu</t>
         </is>
@@ -590,12 +660,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW B</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -603,13 +673,23 @@
       </c>
       <c r="I4" t="n">
         <v>63</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Zhang, ZY (reprint author), Univ Sci &amp; Technol China, Int Ctr Quantum Design Funct Mat ICQD, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Zhang, ZY (reprint author), Univ Sci &amp; Technol China, Synerget Innovat Ctr Quantum Informat &amp; Quantum P, Hefei 230026, Anhui, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Univ Sci &amp; Technol China</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Arif, Suneela</t>
         </is>
@@ -624,19 +704,19 @@
           <t>Ferroelectric and Multiferroic Properties of Single-Phase Yb2NiMnO6 Double-Perovskites</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>suneela.hu@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NEW YORK</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>SPRINGER</t>
+          <t>JOURNAL OF ELECTRONIC MATERIALS</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -644,13 +724,23 @@
       </c>
       <c r="I5" t="n">
         <v>29</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Arif, S (reprint author), Hazara Univ, Dept Phys, Mansehra, Kpk, Pakistan.; Faraz, A (reprint author), UCC, AMSG, Tyndall Natl Inst, Cork, Ireland.</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Hazara Univ</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>Faraz, Ahmad</t>
         </is>
@@ -672,12 +762,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>NEW YORK</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>SPRINGER</t>
+          <t>JOURNAL OF ELECTRONIC MATERIALS</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -685,13 +775,23 @@
       </c>
       <c r="I6" t="n">
         <v>29</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Arif, S (reprint author), Hazara Univ, Dept Phys, Mansehra, Kpk, Pakistan.; Faraz, A (reprint author), UCC, AMSG, Tyndall Natl Inst, Cork, Ireland.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Hazara Univ</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Narayan, Jagdish</t>
         </is>
@@ -713,12 +813,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>OXFORD</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>PERGAMON-ELSEVIER SCIENCE LTD</t>
+          <t>CARBON</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -726,13 +826,23 @@
       </c>
       <c r="I7" t="n">
         <v>73</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Narayan, J (reprint author), North Carolina State Univ, Dept Mat Sci &amp; Engn, Centennial Campus, Raleigh, NC 27695 USA.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>North Carolina State Univ</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Zou, Liangjian</t>
         </is>
@@ -754,12 +864,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF THE AMERICAN CHEMICAL SOCIETY</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -767,13 +877,23 @@
       </c>
       <c r="I8" t="n">
         <v>35</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Chen, XH (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Chen, XH (reprint author), Univ Sci &amp; Technol China, Dept Phys, Hefei 230026, Anhui, Peoples R China.; Chen, XH (reprint author), Univ Sci &amp; Technol China, Key Lab Strongly Coupled Quantum Matter Phys, Hefei 230026, Anhui, Peoples R China.; Zou, LJ (reprint author), Chinese Acad Sci, Inst Solid State Phys, Key Lab Mat Phys, Hefei 230031, Anhui, Peoples R China.; Chen, XH (reprint author), Nanjing Univ, Collaborat Innovat Ctr Adv Microstruct, Nanjing 210093, Jiangsu, Peoples R China.; Chen, XH (reprint author), CAS Ctr Excellence Superconducting Ion CENSE, Shanghai 200050, Peoples R China.; Chen, XH (reprint author), CAS Ctr Excellence Quantum Informat &amp; Quantum Phy, Hefei 230026, Anhui, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Univ Sci &amp; Technol China</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Chen, Xianhui</t>
         </is>
@@ -795,12 +915,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF THE AMERICAN CHEMICAL SOCIETY</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -808,13 +928,23 @@
       </c>
       <c r="I9" t="n">
         <v>35</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Chen, XH (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Chen, XH (reprint author), Univ Sci &amp; Technol China, Dept Phys, Hefei 230026, Anhui, Peoples R China.; Chen, XH (reprint author), Univ Sci &amp; Technol China, Key Lab Strongly Coupled Quantum Matter Phys, Hefei 230026, Anhui, Peoples R China.; Zou, LJ (reprint author), Chinese Acad Sci, Inst Solid State Phys, Key Lab Mat Phys, Hefei 230031, Anhui, Peoples R China.; Chen, XH (reprint author), Nanjing Univ, Collaborat Innovat Ctr Adv Microstruct, Nanjing 210093, Jiangsu, Peoples R China.; Chen, XH (reprint author), CAS Ctr Excellence Superconducting Ion CENSE, Shanghai 200050, Peoples R China.; Chen, XH (reprint author), CAS Ctr Excellence Quantum Informat &amp; Quantum Phy, Hefei 230026, Anhui, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Univ Sci &amp; Technol China</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Sugawara, Akira</t>
         </is>
@@ -836,12 +966,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW MATERIALS</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -849,13 +979,23 @@
       </c>
       <c r="I10" t="n">
         <v>23</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Sugawara, A (reprint author), Hitachi Ltd, Ctr Exploratory Res Lab, Akanuma 2520, Hatoyama, Saitama 3500395, Japan.</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Hitachi Ltd</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>Boldyrev, Alexander, I</t>
         </is>
@@ -877,23 +1017,33 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>PHYSICA STATUS SOLIDI B-BASIC SOLID STATE PHYSICS</t>
         </is>
       </c>
       <c r="I11" t="n">
         <v>57</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Boldyrev, AI (reprint author), Utah State Univ, Dept Chem &amp; Biochem, Logan, UT 84322 USA.</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Utah State Univ</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>Moran-Miguelez, E.</t>
         </is>
@@ -915,12 +1065,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>LAUSANNE</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>ELSEVIER SCIENCE SA</t>
+          <t>JOURNAL OF ALLOYS AND COMPOUNDS</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -928,13 +1078,23 @@
       </c>
       <c r="I12" t="n">
         <v>43</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Moran-Miguelez, E (reprint author), Univ Complutense Madrid, Fac Ciencias Quim, Dept Quim Inorgan, E-28040 Madrid, Spain.</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Univ Complutense Madrid</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Mi, Wenbo</t>
         </is>
@@ -956,23 +1116,33 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>HOBOKEN</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>WILEY</t>
+          <t>ADVANCED ELECTRONIC MATERIALS</t>
         </is>
       </c>
       <c r="I13" t="n">
         <v>50</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Mi, WB (reprint author), Tianjin Univ, Sch Sci, Tianjin Key Lab Low Dimens Mat Phys &amp; Preparat Te, Tianjin 300354, Peoples R China.; Wang, XC (reprint author), Tianjin Univ Technol, Sch Elect &amp; Elect Engn, Tianjin 300384, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Tianjin Univ</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>Wang, Xiaocha</t>
         </is>
@@ -994,23 +1164,33 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>HOBOKEN</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>WILEY</t>
+          <t>ADVANCED ELECTRONIC MATERIALS</t>
         </is>
       </c>
       <c r="I14" t="n">
         <v>50</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Mi, WB (reprint author), Tianjin Univ, Sch Sci, Tianjin Key Lab Low Dimens Mat Phys &amp; Preparat Te, Tianjin 300354, Peoples R China.; Wang, XC (reprint author), Tianjin Univ Technol, Sch Elect &amp; Elect Engn, Tianjin 300384, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Tianjin Univ</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>Zhang Zhen-Hua</t>
         </is>
@@ -1032,12 +1212,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>BEIJING</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>CHINESE PHYSICAL SOC</t>
+          <t>ACTA PHYSICA SINICA</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1045,13 +1225,23 @@
       </c>
       <c r="I15" t="n">
         <v>42</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Zhang, ZH (reprint author), Changsha Univ Sci &amp; Technol, Hunan Prov Key Lab Flexible Elect Mat Genome Engn, Changsha 410114, Hunan, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Changsha Univ Sci &amp; Technol</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>Liu, Kai</t>
         </is>
@@ -1073,12 +1263,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY C</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1086,13 +1276,23 @@
       </c>
       <c r="I16" t="n">
         <v>69</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Liu, K (reprint author), Renmin Univ China, Dept Phys, Beijing 100872, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Renmin Univ China</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>Galbiati, Marta</t>
         </is>
@@ -1114,12 +1314,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW APPLIED</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1127,13 +1327,23 @@
       </c>
       <c r="I17" t="n">
         <v>44</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Galbiati, M (reprint author), Univ Paris Saclay, Univ Paris Sud, CNRS, Unite Mixte Phys,Thales, F-91767 Palaiseau, France.; Galbiati, M (reprint author), Univ Valencia, Inst Ciencia Mol, Catedratico Jose Beltran Martinez 2, Paterna 46980, Spain.</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Univ Paris Saclay</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="3" t="inlineStr">
         <is>
           <t>Dlubak, Bruno</t>
         </is>
@@ -1155,12 +1365,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW APPLIED</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1168,13 +1378,23 @@
       </c>
       <c r="I18" t="n">
         <v>44</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Galbiati, M (reprint author), Univ Paris Saclay, Univ Paris Sud, CNRS, Unite Mixte Phys,Thales, F-91767 Palaiseau, France.; Galbiati, M (reprint author), Univ Valencia, Inst Ciencia Mol, Catedratico Jose Beltran Martinez 2, Paterna 46980, Spain.</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Univ Paris Saclay</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
         <is>
           <t>Seneor, Pierre</t>
         </is>
@@ -1196,12 +1416,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW APPLIED</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1209,20 +1429,30 @@
       </c>
       <c r="I19" t="n">
         <v>44</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Galbiati, M (reprint author), Univ Paris Saclay, Univ Paris Sud, CNRS, Unite Mixte Phys,Thales, F-91767 Palaiseau, France.; Galbiati, M (reprint author), Univ Valencia, Inst Ciencia Mol, Catedratico Jose Beltran Martinez 2, Paterna 46980, Spain.</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Univ Paris Saclay</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Shumskaya, Alena</t>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Shumskaya</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1237,23 +1467,43 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>BELARUS</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>PHYSICA STATUS SOLIDI B-BASIC SOLID STATE PHYSICS</t>
         </is>
       </c>
       <c r="I20" t="n">
         <v>34</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Shumskaya, A (reprint author), NAS Belarus, Sci Pract Mat Res Ctr, Cryogen Div, P Brovki St 19, Minsk 220072, BELARUS.</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>NAS Belarus</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Kaniukov, Egor; Shumskaya, Alena; Kozlovskiy, Artem; Fadeev, Maxim; Rusakov, Vyacheslav; Zdorovets, Maksim</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Shumskaya, A (reprint author), NAS Belarus, Sci Pract Mat Res Ctr, Cryogen Div, P Brovki St 19, Minsk 220072, BELARUS.</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>Han, Ruilin</t>
         </is>
@@ -1275,12 +1525,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1288,13 +1538,23 @@
       </c>
       <c r="I21" t="n">
         <v>50</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Han, RL (reprint author), Shanxi Univ, Sch Phys &amp; Elect Engn, Taiyuan 030006, Shanxi, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Shanxi Univ</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="4" t="inlineStr">
         <is>
           <t>Strauf, Stefan</t>
         </is>
@@ -1316,12 +1576,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>NANO LETTERS</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1329,20 +1589,30 @@
       </c>
       <c r="I22" t="n">
         <v>43</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Strauf, S (reprint author), Stevens Inst Technol, Dept Phys, Hoboken, NJ 07030 USA.; Strauf, S (reprint author), Stevens Inst Technol, Ctr Quantum Sci &amp; Engn, Hoboken, NJ 07030 USA.</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Stevens Inst Technol</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Storchak, Vyacheslav G.</t>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Storchak</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1357,12 +1627,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>OXFORD</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>ELSEVIER SCI LTD</t>
+          <t>MATERIALS TODAY</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1370,13 +1640,33 @@
       </c>
       <c r="I23" t="n">
         <v>37</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Storchak, VG (reprint author), Natl Res Ctr, Kurchatov Inst, Kurchatov Sq 1, Moscow 123182, Russia.</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Natl Res Ctr</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Parfenov, Oleg E.; Tokmachev, Andrey M.; Averyanov, Dmitry, V; Karateev, Igor A.; Sokolov, Ivan S.; Taldenkov, Alexander N.; Storchak, Vyacheslav G.</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Storchak, VG (reprint author), Natl Res Ctr, Kurchatov Inst, Kurchatov Sq 1, Moscow 123182, Russia.</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="4" t="inlineStr">
         <is>
           <t>Hersam, Mark C.</t>
         </is>
@@ -1398,12 +1688,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>LONDON</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>NATURE PUBLISHING GROUP</t>
+          <t>NATURE REVIEWS MATERIALS</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1411,13 +1701,23 @@
       </c>
       <c r="I24" t="n">
         <v>225</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Hersam, MC (reprint author), Northwestern Univ, Appl Phys Grad Program, Evanston, IL 60208 USA.; Hersam, MC (reprint author), Northwestern Univ, Dept Mat Sci &amp; Engn, Evanston, IL 60208 USA.; Hersam, MC (reprint author), Northwestern Univ, Dept Chem, Evanston, IL 60208 USA.; Hersam, MC (reprint author), Northwestern Univ, Dept Elect &amp; Comp Engn, Evanston, IL 60208 USA.</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Northwestern Univ</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>Rahman, Altaf Ur</t>
         </is>
@@ -1432,19 +1732,19 @@
           <t>Robust ferromagnetism and half-metallicity in hydrogenated monolayer-CdS</t>
         </is>
       </c>
-      <c r="E25" s="2" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>altafqau1@gmail.com</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>ELSEVIER</t>
+          <t>PHYSICA B-CONDENSED MATTER</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1452,20 +1752,30 @@
       </c>
       <c r="I25" t="n">
         <v>39</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Rahman, AU (reprint author), Int Islamic Univ, Dept Phys, Islamabad 44000, Pakistan.</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Int Islamic Univ</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Ullah, Hameed</t>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Ullah</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1473,19 +1783,19 @@
           <t>Robust ferromagnetism and half-metallicity in hydrogenated monolayer-CdS</t>
         </is>
       </c>
-      <c r="E26" s="2" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>hameedktk331@gmail.com</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>ELSEVIER</t>
+          <t>PHYSICA B-CONDENSED MATTER</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1493,13 +1803,33 @@
       </c>
       <c r="I26" t="n">
         <v>39</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Rahman, AU (reprint author), Int Islamic Univ, Dept Phys, Islamabad 44000, Pakistan.</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Int Islamic Univ</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Rahman, Altaf Ur; Ullah, Hameed; Jamil, Asif; Iqbal, Zahid; Naveed-Ul-Haq, M.</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Rahman, AU (reprint author), Int Islamic Univ, Dept Phys, Islamabad 44000, Pakistan.</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>Naveed-Ul-Haq, M.</t>
         </is>
@@ -1521,12 +1851,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>ELSEVIER</t>
+          <t>PHYSICA B-CONDENSED MATTER</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1534,13 +1864,23 @@
       </c>
       <c r="I27" t="n">
         <v>39</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Rahman, AU (reprint author), Int Islamic Univ, Dept Phys, Islamabad 44000, Pakistan.</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Int Islamic Univ</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="3" t="inlineStr">
         <is>
           <t>Olsen, Thomas</t>
         </is>
@@ -1562,12 +1902,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>2D MATERIALS</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1575,13 +1915,23 @@
       </c>
       <c r="I28" t="n">
         <v>53</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Olsen, T (reprint author), Tech Univ Denmark, Computat Atom Scale Mat Design CAMD, Dept Phys, DK-2800 Lyngby, Denmark.</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Tech Univ Denmark</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="3" t="inlineStr">
         <is>
           <t>Boldyrev, Alexander, I</t>
         </is>
@@ -1603,12 +1953,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1616,13 +1966,23 @@
       </c>
       <c r="I29" t="n">
         <v>70</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Boldyrev, AI (reprint author), Utah State Univ, Dept Chem &amp; Biochem, Logan, UT 84322 USA.; Boldyrev, AI (reprint author), Southern Fed Univ, Inst Phys &amp; Organ Chem, 194-2 Stachka Ave, Rostov Na Donu 344090, Russia.</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Utah State Univ</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>Cui, Bin</t>
         </is>
@@ -1644,12 +2004,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -1657,13 +2017,23 @@
       </c>
       <c r="I30" t="n">
         <v>28</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Cui, B; Liu, DS (reprint author), Shandong Univ, Sch Phys, State Key Lab Crystal Mat, Jinan 250100, Shandong, Peoples R China.; Liu, DS (reprint author), Jining Univ, Dept Phys, Qufu 273155, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>DS (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>Liu, Desheng</t>
         </is>
@@ -1685,12 +2055,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -1698,13 +2068,23 @@
       </c>
       <c r="I31" t="n">
         <v>28</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Cui, B; Liu, DS (reprint author), Shandong Univ, Sch Phys, State Key Lab Crystal Mat, Jinan 250100, Shandong, Peoples R China.; Liu, DS (reprint author), Jining Univ, Dept Phys, Qufu 273155, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>DS (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>Li, Yu</t>
         </is>
@@ -1726,12 +2106,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>ELSEVIER SCIENCE BV</t>
+          <t>APPLIED SURFACE SCIENCE</t>
         </is>
       </c>
       <c r="H32" t="n">
@@ -1739,13 +2119,23 @@
       </c>
       <c r="I32" t="n">
         <v>59</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Li, Y (reprint author), Shenzhen Univ, Coll Mat Sci &amp; Engn, Shenzhen Key Lab Special Funct Mat, Shenzhen 518060, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Shenzhen Univ</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
         <is>
           <t>Feng, Baojie</t>
         </is>
@@ -1767,12 +2157,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW LETTERS</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -1780,20 +2170,30 @@
       </c>
       <c r="I33" t="n">
         <v>29</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Feng, BJ (reprint author), Chinese Acad Sci, Inst Phys, Beijing 100190, Peoples R China.; Feng, BJ (reprint author), Hiroshima Univ, Hiroshima Synchrotron Radiat Ctr, 2-313 Kagamiyama, Higashihiroshima 7390046, Japan.; Feng, BJ (reprint author), Univ Chinese Acad Sci, Sch Phys Sci, Beijing 100049, Peoples R China.; Yao, YG (reprint author), Beijing Inst Technol, Key Lab Adv Optoelect Quantum Architecture &amp; Meas, Beijing Key Lab Nanophoton Ultrafine Optoelect Sy, Beijing 100081, Peoples R China.; Yao, YG (reprint author), Beijing Inst Technol, Sch Phys, Beijing 100081, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Chinese Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Feng, Ya</t>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>Yao, Yugui</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Feng</t>
+          <t>Yao</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1808,12 +2208,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW LETTERS</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -1821,13 +2221,23 @@
       </c>
       <c r="I34" t="n">
         <v>29</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Feng, BJ (reprint author), Chinese Acad Sci, Inst Phys, Beijing 100190, Peoples R China.; Feng, BJ (reprint author), Hiroshima Univ, Hiroshima Synchrotron Radiat Ctr, 2-313 Kagamiyama, Higashihiroshima 7390046, Japan.; Feng, BJ (reprint author), Univ Chinese Acad Sci, Sch Phys Sci, Beijing 100049, Peoples R China.; Yao, YG (reprint author), Beijing Inst Technol, Key Lab Adv Optoelect Quantum Architecture &amp; Meas, Beijing Key Lab Nanophoton Ultrafine Optoelect Sy, Beijing 100081, Peoples R China.; Yao, YG (reprint author), Beijing Inst Technol, Sch Phys, Beijing 100081, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Chinese Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>Luo, X.</t>
         </is>
@@ -1849,12 +2259,12 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW B</t>
         </is>
       </c>
       <c r="H35" t="n">
@@ -1862,13 +2272,23 @@
       </c>
       <c r="I35" t="n">
         <v>56</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Luo, X (reprint author), Chinese Acad Sci, Inst Solid State Phys, Key Lab Mat Phys, Hefei 230031, Anhui, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Chinese Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="2" t="inlineStr">
         <is>
           <t>Sun, Y. P.</t>
         </is>
@@ -1890,12 +2310,12 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW B</t>
         </is>
       </c>
       <c r="H36" t="n">
@@ -1903,13 +2323,23 @@
       </c>
       <c r="I36" t="n">
         <v>56</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Luo, X (reprint author), Chinese Acad Sci, Inst Solid State Phys, Key Lab Mat Phys, Hefei 230031, Anhui, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Chinese Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>Guo, Chunsheng</t>
         </is>
@@ -1931,12 +2361,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>ELSEVIER</t>
+          <t>APPLIED SURFACE SCIENCE</t>
         </is>
       </c>
       <c r="H37" t="n">
@@ -1944,13 +2374,23 @@
       </c>
       <c r="I37" t="n">
         <v>46</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Zhao, Y (reprint author), Southwest Jiaotong Univ, Superconduct &amp; New Energy R&amp;D Ctr, Key Lab Magnet Levitat Technol &amp; Maglev Trains, Minist Educ, Mail Stop 165, Chengdu 610031, Sichuan, Peoples R China.; Guo, CS (reprint author), Southwest Jiaotong Univ, Superconduct &amp; New Energy R&amp;D Ctr, Key Lab Adv Technol Mat, Minist Educ, Mail Stop 165, Chengdu 610031, Sichuan, Peoples R China.; Shi, XQ (reprint author), Southern Univ Sci &amp; Technol, Dept Phys, Shenzhen 518055, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Southwest Jiaotong Univ</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="2" t="inlineStr">
         <is>
           <t>Shi, Xingqiang</t>
         </is>
@@ -1972,12 +2412,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>ELSEVIER</t>
+          <t>APPLIED SURFACE SCIENCE</t>
         </is>
       </c>
       <c r="H38" t="n">
@@ -1985,13 +2425,23 @@
       </c>
       <c r="I38" t="n">
         <v>46</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Zhao, Y (reprint author), Southwest Jiaotong Univ, Superconduct &amp; New Energy R&amp;D Ctr, Key Lab Magnet Levitat Technol &amp; Maglev Trains, Minist Educ, Mail Stop 165, Chengdu 610031, Sichuan, Peoples R China.; Guo, CS (reprint author), Southwest Jiaotong Univ, Superconduct &amp; New Energy R&amp;D Ctr, Key Lab Adv Technol Mat, Minist Educ, Mail Stop 165, Chengdu 610031, Sichuan, Peoples R China.; Shi, XQ (reprint author), Southern Univ Sci &amp; Technol, Dept Phys, Shenzhen 518055, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Southwest Jiaotong Univ</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>Zhao, Yong</t>
         </is>
@@ -2013,12 +2463,12 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>ELSEVIER</t>
+          <t>APPLIED SURFACE SCIENCE</t>
         </is>
       </c>
       <c r="H39" t="n">
@@ -2026,13 +2476,23 @@
       </c>
       <c r="I39" t="n">
         <v>46</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Zhao, Y (reprint author), Southwest Jiaotong Univ, Superconduct &amp; New Energy R&amp;D Ctr, Key Lab Magnet Levitat Technol &amp; Maglev Trains, Minist Educ, Mail Stop 165, Chengdu 610031, Sichuan, Peoples R China.; Guo, CS (reprint author), Southwest Jiaotong Univ, Superconduct &amp; New Energy R&amp;D Ctr, Key Lab Adv Technol Mat, Minist Educ, Mail Stop 165, Chengdu 610031, Sichuan, Peoples R China.; Shi, XQ (reprint author), Southern Univ Sci &amp; Technol, Dept Phys, Shenzhen 518055, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Southwest Jiaotong Univ</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="4" t="inlineStr">
         <is>
           <t>Chen, Zhongfang</t>
         </is>
@@ -2047,19 +2507,19 @@
           <t>Oxygen Evolution Reaction on 2D Ferromagnetic Fe3GeTe2: Boosting the Reactivity by the Self-Reduction of Surface Hydroxyl</t>
         </is>
       </c>
-      <c r="E40" s="2" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>zhongfangchen@gmail.com</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED FUNCTIONAL MATERIALS</t>
         </is>
       </c>
       <c r="H40" t="n">
@@ -2067,20 +2527,30 @@
       </c>
       <c r="I40" t="n">
         <v>91</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Chen, ZF (reprint author), Univ Puerto Rico, Dept Chem, San Juan, PR 00931 USA.</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Univ Puerto Rico</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Loh, Kian Ping</t>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Loh</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2095,12 +2565,12 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -2108,13 +2578,33 @@
       </c>
       <c r="I41" t="n">
         <v>32</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Loh, KP (reprint author), Natl Univ Singapore, Dept Chem, 3 Sci Dr 3, Singapore 117543, Singapore.; Loh, KP (reprint author), Natl Univ Singapore, Ctr Adv 2D Mat, Singapore 117546, Singapore.</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Natl Univ Singapore</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Yu, Wei; Li, Jing; Herng, Tun Seng; Wang, Zishen; Zhao, Xiaoxu; Chi, Xiao; Fu, Wei; Abdelwahab, Ibrahim; Zhou, Jun; Dan, Jiadong; Chen, Zhongxin; Chen, Zhi; Li, Zejun; Lu, Jiong; Pennycook, Stephen J.; Feng, Yuan Ping; Ding, Jun; Loh, Kian Ping</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Loh, KP (reprint author), Natl Univ Singapore, Dept Chem, 3 Sci Dr 3, Singapore 117543, Singapore.; Loh, KP (reprint author), Natl Univ Singapore, Ctr Adv 2D Mat, Singapore 117546, Singapore.</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="3" t="inlineStr">
         <is>
           <t>Zollner, Klaus</t>
         </is>
@@ -2136,12 +2626,12 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW B</t>
         </is>
       </c>
       <c r="H42" t="n">
@@ -2149,13 +2639,23 @@
       </c>
       <c r="I42" t="n">
         <v>111</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Zollner, K (reprint author), Univ Regensburg, Inst Theoret Phys, D-93040 Regensburg, Germany.</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Univ Regensburg</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>Sheng, Xian-Lei</t>
         </is>
@@ -2177,12 +2677,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW MATERIALS</t>
         </is>
       </c>
       <c r="H43" t="n">
@@ -2190,20 +2690,30 @@
       </c>
       <c r="I43" t="n">
         <v>53</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Sheng, XL (reprint author), Singapore Univ Technol &amp; Design, Res Lab Quantum Mat, Singapore 487372, Singapore.; Sheng, XL (reprint author), Beihang Univ, Minist Educ, Key Lab Micronano Measurement Manipulat &amp; Phys, Dept Phys, Beijing 100191, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Singapore Univ Technol &amp; Design</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Yang, Shengyuan A.</t>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>Sheng, Xian-Lei</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Yang</t>
+          <t>Sheng</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2218,12 +2728,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW MATERIALS</t>
         </is>
       </c>
       <c r="H44" t="n">
@@ -2231,13 +2741,23 @@
       </c>
       <c r="I44" t="n">
         <v>53</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Sheng, XL (reprint author), Singapore Univ Technol &amp; Design, Res Lab Quantum Mat, Singapore 487372, Singapore.; Sheng, XL (reprint author), Beihang Univ, Minist Educ, Key Lab Micronano Measurement Manipulat &amp; Phys, Dept Phys, Beijing 100191, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Singapore Univ Technol &amp; Design</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="5" t="inlineStr">
         <is>
           <t>Zoppellaro, Giorgio</t>
         </is>
@@ -2252,19 +2772,19 @@
           <t>Microwave Energy Drives "On-Off-On" Spin-Switch Behavior in Nitrogen-Doped Graphene</t>
         </is>
       </c>
-      <c r="E45" s="2" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>zoppellarogiorgio@gmail.com</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>Republic</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H45" t="n">
@@ -2272,13 +2792,23 @@
       </c>
       <c r="I45" t="n">
         <v>74</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Zoppellaro, G; Zboril, R (reprint author), Palacky Univ Olomouc, Fac Sci, Reg Ctr Adv Technol &amp; Mat, Dept Phys Chem, Slechtitelu 27, Olomouc 78371, Czech Republic.</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>R (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="5" t="inlineStr">
         <is>
           <t>Zboril, Radek</t>
         </is>
@@ -2300,12 +2830,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>Republic</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H46" t="n">
@@ -2313,15 +2843,25 @@
       </c>
       <c r="I46" t="n">
         <v>74</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Zoppellaro, G; Zboril, R (reprint author), Palacky Univ Olomouc, Fac Sci, Reg Ctr Adv Technol &amp; Mat, Dept Phys Chem, Slechtitelu 27, Olomouc 78371, Czech Republic.</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>R (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Li, Xiangyang</t>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>Li, Xingxing</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2341,12 +2881,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY LETTERS</t>
         </is>
       </c>
       <c r="H47" t="n">
@@ -2354,13 +2894,23 @@
       </c>
       <c r="I47" t="n">
         <v>25</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Li, XX; Yang, JL (reprint author), Univ Sci &amp; Technol China, Synerget Innovat Ctr Quantum Informat &amp; Quantum P, Hefei 230026, Anhui, Peoples R China.; Yang, JL (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Li, XX; Yang, JL (reprint author), Univ Sci &amp; Technol China, Dept Chem Phys, Hefei 230026, Anhui, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>JL (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="2" t="inlineStr">
         <is>
           <t>Yang, Jinlong</t>
         </is>
@@ -2382,12 +2932,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY LETTERS</t>
         </is>
       </c>
       <c r="H48" t="n">
@@ -2395,13 +2945,23 @@
       </c>
       <c r="I48" t="n">
         <v>25</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Li, XX; Yang, JL (reprint author), Univ Sci &amp; Technol China, Synerget Innovat Ctr Quantum Informat &amp; Quantum P, Hefei 230026, Anhui, Peoples R China.; Yang, JL (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Li, XX; Yang, JL (reprint author), Univ Sci &amp; Technol China, Dept Chem Phys, Hefei 230026, Anhui, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>JL (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="3" t="inlineStr">
         <is>
           <t>Kakazei, G. N.</t>
         </is>
@@ -2423,12 +2983,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>MELVILLE</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>AMER INST PHYSICS</t>
+          <t>APL MATERIALS</t>
         </is>
       </c>
       <c r="H49" t="n">
@@ -2436,13 +2996,23 @@
       </c>
       <c r="I49" t="n">
         <v>41</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Kakazei, GN (reprint author), Univ Porto, Dept Fis &amp; Astron, Inst Phys Adv Mat Nanotechnol &amp; Photon IFIMUP, P-4169007 Porto, Portugal.</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Univ Porto</t>
+        </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="3" t="inlineStr">
         <is>
           <t>Hinov, Nikolay</t>
         </is>
@@ -2464,12 +3034,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>NOVI PAZAR</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>ASSOC INFORMATION COMMUNICATION TECHNOLOGY EDUCATION &amp; SCIENCE</t>
+          <t>TEM JOURNAL-TECHNOLOGY EDUCATION MANAGEMENT INFORMATICS</t>
         </is>
       </c>
       <c r="H50" t="n">
@@ -2477,13 +3047,23 @@
       </c>
       <c r="I50" t="n">
         <v>18</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Hinov, N (reprint author), Tech Univ Sofia, Fac Elect Engn &amp; Technol, 8 Kliment Ohridski Blvd, Sofia 1000, Bulgaria.</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Tech Univ Sofia</t>
+        </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="3" t="inlineStr">
         <is>
           <t>Basu, Tathamay</t>
         </is>
@@ -2505,12 +3085,12 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED FUNCTIONAL MATERIALS</t>
         </is>
       </c>
       <c r="H51" t="n">
@@ -2518,13 +3098,23 @@
       </c>
       <c r="I51" t="n">
         <v>55</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Basu, T; Raveau, B (reprint author), Normandie Univ, ENSICAEN, UNICAEN, CNRS,CRISMAT, 6 Bd Marechal Juin, F-14050 Caen, France.</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>B (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B52" s="3" t="inlineStr">
         <is>
           <t>Raveau, Bernard</t>
         </is>
@@ -2546,12 +3136,12 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED FUNCTIONAL MATERIALS</t>
         </is>
       </c>
       <c r="H52" t="n">
@@ -2559,13 +3149,23 @@
       </c>
       <c r="I52" t="n">
         <v>55</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Basu, T; Raveau, B (reprint author), Normandie Univ, ENSICAEN, UNICAEN, CNRS,CRISMAT, 6 Bd Marechal Juin, F-14050 Caen, France.</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>B (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B53" s="2" t="inlineStr">
         <is>
           <t>Dietl, Tomasz</t>
         </is>
@@ -2587,12 +3187,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>JOURNAL OF SEMICONDUCTORS</t>
         </is>
       </c>
       <c r="H53" t="n">
@@ -2600,13 +3200,23 @@
       </c>
       <c r="I53" t="n">
         <v>87</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Dietl, T (reprint author), Polish Acad Sci, Inst Phys, Int Res Ctr MagTop, Aleja Lotnikow 32-46, PL-02668 Warsaw, Poland.; Dietl, T; Ohno, H (reprint author), Tohoku Univ, WPI Adv Inst Mat Res, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Bonanni, A (reprint author), Johannes Kepler Univ Linz, Inst Halbleiter &amp; Festkorperphys, Altenbergerstr 69, A-4040 Linz, Austria.; Ohno, H (reprint author), Tohoku Univ, Elect Commun Res Inst, Lab Nanoelect &amp; Spintron, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Sci &amp; Innovat Spintron, Core Res Cluster, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Spintron Integrated Syst, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Innovat Integrated Elect Syst, Aoba Ku, 468-1 Aramaki Aza Aoba, Sendai, Miyagi 9800845, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Spintron Res Network, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Polish Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" s="2" t="inlineStr">
         <is>
           <t>Bonanni, Alberta</t>
         </is>
@@ -2628,12 +3238,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>JOURNAL OF SEMICONDUCTORS</t>
         </is>
       </c>
       <c r="H54" t="n">
@@ -2641,13 +3251,23 @@
       </c>
       <c r="I54" t="n">
         <v>87</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Dietl, T (reprint author), Polish Acad Sci, Inst Phys, Int Res Ctr MagTop, Aleja Lotnikow 32-46, PL-02668 Warsaw, Poland.; Dietl, T; Ohno, H (reprint author), Tohoku Univ, WPI Adv Inst Mat Res, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Bonanni, A (reprint author), Johannes Kepler Univ Linz, Inst Halbleiter &amp; Festkorperphys, Altenbergerstr 69, A-4040 Linz, Austria.; Ohno, H (reprint author), Tohoku Univ, Elect Commun Res Inst, Lab Nanoelect &amp; Spintron, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Sci &amp; Innovat Spintron, Core Res Cluster, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Spintron Integrated Syst, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Innovat Integrated Elect Syst, Aoba Ku, 468-1 Aramaki Aza Aoba, Sendai, Miyagi 9800845, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Spintron Res Network, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Polish Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="2" t="inlineStr">
         <is>
           <t>Ohno, Hideo</t>
         </is>
@@ -2669,12 +3289,12 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>JOURNAL OF SEMICONDUCTORS</t>
         </is>
       </c>
       <c r="H55" t="n">
@@ -2682,20 +3302,30 @@
       </c>
       <c r="I55" t="n">
         <v>87</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Dietl, T (reprint author), Polish Acad Sci, Inst Phys, Int Res Ctr MagTop, Aleja Lotnikow 32-46, PL-02668 Warsaw, Poland.; Dietl, T; Ohno, H (reprint author), Tohoku Univ, WPI Adv Inst Mat Res, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Bonanni, A (reprint author), Johannes Kepler Univ Linz, Inst Halbleiter &amp; Festkorperphys, Altenbergerstr 69, A-4040 Linz, Austria.; Ohno, H (reprint author), Tohoku Univ, Elect Commun Res Inst, Lab Nanoelect &amp; Spintron, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Sci &amp; Innovat Spintron, Core Res Cluster, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Spintron Integrated Syst, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Innovat Integrated Elect Syst, Aoba Ku, 468-1 Aramaki Aza Aoba, Sendai, Miyagi 9800845, Japan.; Ohno, H (reprint author), Tohoku Univ, Ctr Spintron Res Network, Aoba Ku, 2-1-1 Katahira, Sendai, Miyagi 9808577, Japan.</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Polish Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Xia, Congxin</t>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>Wei, Zhongming</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Xia</t>
+          <t>Wei</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2710,12 +3340,12 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>JOURNAL OF SEMICONDUCTORS</t>
         </is>
       </c>
       <c r="H56" t="n">
@@ -2723,20 +3353,30 @@
       </c>
       <c r="I56" t="n">
         <v>59</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Xia, CX (reprint author), Henan Normal Univ, Dept Phys, Xinxiang 453007, Henan, Peoples R China.; Wei, ZM (reprint author), Chinese Acad Sci, Inst Semicond, Beijing 100083, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Henan Normal Univ</t>
+        </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Wei, Zhongming</t>
+      <c r="B57" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Wei</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2751,12 +3391,12 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>JOURNAL OF SEMICONDUCTORS</t>
         </is>
       </c>
       <c r="H57" t="n">
@@ -2764,13 +3404,33 @@
       </c>
       <c r="I57" t="n">
         <v>59</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Xia, CX (reprint author), Henan Normal Univ, Dept Phys, Xinxiang 453007, Henan, Peoples R China.; Wei, ZM (reprint author), Chinese Acad Sci, Inst Semicond, Beijing 100083, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Henan Normal Univ</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Zhai, Baoxing; Du, Juan; Li, Xueping; Xia, Congxin; Wei, Zhongming</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Xia, CX (reprint author), Henan Normal Univ, Dept Phys, Xinxiang 453007, Henan, Peoples R China.; Wei, ZM (reprint author), Chinese Acad Sci, Inst Semicond, Beijing 100083, Peoples R China.</t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B58" s="4" t="inlineStr">
         <is>
           <t>Goldberger, Joshua E.</t>
         </is>
@@ -2792,12 +3452,12 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>NANO LETTERS</t>
         </is>
       </c>
       <c r="H58" t="n">
@@ -2805,20 +3465,30 @@
       </c>
       <c r="I58" t="n">
         <v>27</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Goldberger, JE (reprint author), Ohio State Univ, Dept Chem &amp; Biochem, Columbus, OH 43210 USA.</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Ohio State Univ</t>
+        </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Wang, Shengping</t>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Wang</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2833,12 +3503,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>PHYSICA STATUS SOLIDI B-BASIC SOLID STATE PHYSICS</t>
         </is>
       </c>
       <c r="H59" t="n">
@@ -2846,13 +3516,33 @@
       </c>
       <c r="I59" t="n">
         <v>37</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Xu, MS (reprint author), Zhejiang Univ, State Key Lab Silicon Mat, Coll Informat Sci &amp; Elect Engn, Hangzhou 310027, Zhejiang, Peoples R China.; Pi, XD (reprint author), Zhejiang Univ, Sch Mat Sci &amp; Engn, State Key Lab Silicon Mat, Hangzhou 310027, Zhejiang, Peoples R China.; Xu, MS (reprint author), Guizhou Univ, Coll Big Data &amp; Informat Engn, Guiyang 550025, Guizhou, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Zhejiang Univ</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Habib, Mohammad R.; Wang, Shengping; Obaidulla, Sk M.; Khan, Yahya; Pi, Xiaodong; Xu, Mingsheng</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Xu, MS (reprint author), Zhejiang Univ, State Key Lab Silicon Mat, Coll Informat Sci &amp; Elect Engn, Hangzhou 310027, Zhejiang, Peoples R China.; Pi, XD (reprint author), Zhejiang Univ, Sch Mat Sci &amp; Engn, State Key Lab Silicon Mat, Hangzhou 310027, Zhejiang, Peoples R China.; Xu, MS (reprint author), Guizhou Univ, Coll Big Data &amp; Informat Engn, Guiyang 550025, Guizhou, Peoples R China.</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B60" s="2" t="inlineStr">
         <is>
           <t>Xu, Mingsheng</t>
         </is>
@@ -2874,12 +3564,12 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>PHYSICA STATUS SOLIDI B-BASIC SOLID STATE PHYSICS</t>
         </is>
       </c>
       <c r="H60" t="n">
@@ -2887,13 +3577,23 @@
       </c>
       <c r="I60" t="n">
         <v>37</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Xu, MS (reprint author), Zhejiang Univ, State Key Lab Silicon Mat, Coll Informat Sci &amp; Elect Engn, Hangzhou 310027, Zhejiang, Peoples R China.; Pi, XD (reprint author), Zhejiang Univ, Sch Mat Sci &amp; Engn, State Key Lab Silicon Mat, Hangzhou 310027, Zhejiang, Peoples R China.; Xu, MS (reprint author), Guizhou Univ, Coll Big Data &amp; Informat Engn, Guiyang 550025, Guizhou, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Zhejiang Univ</t>
+        </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B61" s="4" t="inlineStr">
         <is>
           <t>Zhuang, Houlong L.</t>
         </is>
@@ -2915,12 +3615,12 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>ELSEVIER</t>
+          <t>COMPUTATIONAL MATERIALS SCIENCE</t>
         </is>
       </c>
       <c r="H61" t="n">
@@ -2928,20 +3628,30 @@
       </c>
       <c r="I61" t="n">
         <v>41</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Zhuang, HL (reprint author), Arizona State Univ, Sch Engn Matter Transport &amp; Energy, Tempe, AZ 85287 USA.</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Arizona State Univ</t>
+        </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Tian, Shangjie</t>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>Zhang, Xiao</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Tian</t>
+          <t>Zhang</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2956,12 +3666,12 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>BEIJING</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>HIGHER EDUCATION PRESS</t>
+          <t>FRONTIERS OF PHYSICS</t>
         </is>
       </c>
       <c r="H62" t="n">
@@ -2969,13 +3679,23 @@
       </c>
       <c r="I62" t="n">
         <v>20</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Zhang, X (reprint author), Beijing Univ Posts &amp; Telecommun, State Key Lab Informat Photon &amp; Opt Commun, Beijing 100876, Peoples R China.; Zhang, X (reprint author), Beijing Univ Posts &amp; Telecommun, Sch Sci, Beijing 100876, Peoples R China.; Lei, HC (reprint author), Renmin Univ China, Dept Phys, Beijing 100872, Peoples R China.; Lei, HC (reprint author), Renmin Univ China, Beijing Key Lab Optoelect Funct Mat &amp; Micronano D, Beijing 100872, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Beijing Univ Posts &amp; Telecommun</t>
+        </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B63" s="2" t="inlineStr">
         <is>
           <t>Lei, Hechang</t>
         </is>
@@ -2997,12 +3717,12 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>BEIJING</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>HIGHER EDUCATION PRESS</t>
+          <t>FRONTIERS OF PHYSICS</t>
         </is>
       </c>
       <c r="H63" t="n">
@@ -3010,13 +3730,23 @@
       </c>
       <c r="I63" t="n">
         <v>20</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Zhang, X (reprint author), Beijing Univ Posts &amp; Telecommun, State Key Lab Informat Photon &amp; Opt Commun, Beijing 100876, Peoples R China.; Zhang, X (reprint author), Beijing Univ Posts &amp; Telecommun, Sch Sci, Beijing 100876, Peoples R China.; Lei, HC (reprint author), Renmin Univ China, Dept Phys, Beijing 100872, Peoples R China.; Lei, HC (reprint author), Renmin Univ China, Beijing Key Lab Optoelect Funct Mat &amp; Micronano D, Beijing 100872, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Beijing Univ Posts &amp; Telecommun</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B64" s="2" t="inlineStr">
         <is>
           <t>Dai, Lun</t>
         </is>
@@ -3038,12 +3768,12 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>HOBOKEN</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>WILEY</t>
+          <t>ADVANCED ELECTRONIC MATERIALS</t>
         </is>
       </c>
       <c r="H64" t="n">
@@ -3051,13 +3781,23 @@
       </c>
       <c r="I64" t="n">
         <v>32</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Dai, L; Ye, Y (reprint author), Peking Univ, State Key Lab Artificial Microstruct &amp; Mesoscop P, Beijing 100871, Peoples R China.; Dai, L; Ye, Y (reprint author), Peking Univ, Sch Phys, Beijing 100871, Peoples R China.; Dai, L; Ye, Y (reprint author), Collaborat Innovat Ctr Quantum Matter, Beijing 100871, Peoples R China.; Zhao, JH (reprint author), Chinese Acad Sci, Inst Semicond, State Key Lab Superlattices &amp; Microstruct, Beijing 100083, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Y (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B65" s="2" t="inlineStr">
         <is>
           <t>Zhao, Jianhua</t>
         </is>
@@ -3079,12 +3819,12 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>HOBOKEN</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>WILEY</t>
+          <t>ADVANCED ELECTRONIC MATERIALS</t>
         </is>
       </c>
       <c r="H65" t="n">
@@ -3092,13 +3832,23 @@
       </c>
       <c r="I65" t="n">
         <v>32</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Dai, L; Ye, Y (reprint author), Peking Univ, State Key Lab Artificial Microstruct &amp; Mesoscop P, Beijing 100871, Peoples R China.; Dai, L; Ye, Y (reprint author), Peking Univ, Sch Phys, Beijing 100871, Peoples R China.; Dai, L; Ye, Y (reprint author), Collaborat Innovat Ctr Quantum Matter, Beijing 100871, Peoples R China.; Zhao, JH (reprint author), Chinese Acad Sci, Inst Semicond, State Key Lab Superlattices &amp; Microstruct, Beijing 100083, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Y (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B66" s="2" t="inlineStr">
         <is>
           <t>Ye, Yu</t>
         </is>
@@ -3120,12 +3870,12 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>HOBOKEN</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>WILEY</t>
+          <t>ADVANCED ELECTRONIC MATERIALS</t>
         </is>
       </c>
       <c r="H66" t="n">
@@ -3133,20 +3883,30 @@
       </c>
       <c r="I66" t="n">
         <v>32</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Dai, L; Ye, Y (reprint author), Peking Univ, State Key Lab Artificial Microstruct &amp; Mesoscop P, Beijing 100871, Peoples R China.; Dai, L; Ye, Y (reprint author), Peking Univ, Sch Phys, Beijing 100871, Peoples R China.; Dai, L; Ye, Y (reprint author), Collaborat Innovat Ctr Quantum Matter, Beijing 100871, Peoples R China.; Zhao, JH (reprint author), Chinese Acad Sci, Inst Semicond, State Key Lab Superlattices &amp; Microstruct, Beijing 100083, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Y (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Huang, Chengxi</t>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Huang</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3154,19 +3914,19 @@
           <t>Boosting the Curie Temperature of Two-Dimensional Semiconducting Crl(3) Monolayer through van der Waals Heterostructures</t>
         </is>
       </c>
-      <c r="E67" s="2" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>dawnhcx@gmail.com</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY C</t>
         </is>
       </c>
       <c r="H67" t="n">
@@ -3174,13 +3934,33 @@
       </c>
       <c r="I67" t="n">
         <v>45</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Dept Appl Phys, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Inst Energy &amp; Microstruct, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Jena, P (reprint author), Virginia Commonwealth Univ, Dept Phys, Richmond, VA 23284 USA.</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>EJ (reprint author)</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Chen, Shanbao; Huang, Chengxi; Sun, Huasheng; Ding, Junfei; Jena, Puru; Kan, Erjun</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Dept Appl Phys, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Inst Energy &amp; Microstruct, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Jena, P (reprint author), Virginia Commonwealth Univ, Dept Phys, Richmond, VA 23284 USA.</t>
+        </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B68" s="4" t="inlineStr">
         <is>
           <t>Jena, Puru</t>
         </is>
@@ -3202,12 +3982,12 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY C</t>
         </is>
       </c>
       <c r="H68" t="n">
@@ -3215,13 +3995,23 @@
       </c>
       <c r="I68" t="n">
         <v>45</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Dept Appl Phys, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Inst Energy &amp; Microstruct, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Jena, P (reprint author), Virginia Commonwealth Univ, Dept Phys, Richmond, VA 23284 USA.</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>EJ (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B69" s="4" t="inlineStr">
         <is>
           <t>Kan, Erjun</t>
         </is>
@@ -3243,12 +4033,12 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY C</t>
         </is>
       </c>
       <c r="H69" t="n">
@@ -3256,15 +4046,25 @@
       </c>
       <c r="I69" t="n">
         <v>45</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Dept Appl Phys, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Kan, EJ (reprint author), Nanjing Univ Sci &amp; Technol, Inst Energy &amp; Microstruct, Nanjing 210094, Jiangsu, Peoples R China.; Huang, CX; Jena, P (reprint author), Virginia Commonwealth Univ, Dept Phys, Richmond, VA 23284 USA.</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>EJ (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Wang, Haiyan</t>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>Wang, Han</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3284,12 +4084,12 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>ACS APPLIED MATERIALS &amp; INTERFACES</t>
         </is>
       </c>
       <c r="H70" t="n">
@@ -3297,13 +4097,23 @@
       </c>
       <c r="I70" t="n">
         <v>42</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Wang, HY (reprint author), Purdue Univ, Sch Mat Engn, W Lafayette, IN 47907 USA.; Wang, HY (reprint author), Purdue Univ, Sch Elect &amp; Comp Engn, W Lafayette, IN 47907 USA.</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Purdue Univ</t>
+        </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B71" s="2" t="inlineStr">
         <is>
           <t>Gao, Junfeng</t>
         </is>
@@ -3325,12 +4135,12 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW MATERIALS</t>
         </is>
       </c>
       <c r="H71" t="n">
@@ -3338,20 +4148,30 @@
       </c>
       <c r="I71" t="n">
         <v>62</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Gao, JF (reprint author), Dalian Univ Technol, Minist Educ, Lab Mat Modificat Laser Ion &amp; Electron Beams, Dalian 116024, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Dalian Univ Technol</t>
+        </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Zhang, Shengli</t>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Zhang</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3366,12 +4186,12 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW MATERIALS</t>
         </is>
       </c>
       <c r="H72" t="n">
@@ -3379,13 +4199,33 @@
       </c>
       <c r="I72" t="n">
         <v>62</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Gao, JF (reprint author), Dalian Univ Technol, Minist Educ, Lab Mat Modificat Laser Ion &amp; Electron Beams, Dalian 116024, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Dalian Univ Technol</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Hu, Ziyu; Gao, Junfeng; Zhang, Shengli; Zhao, Jijun; Zhou, Wenhan; Zeng, Haibo</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>Gao, JF (reprint author), Dalian Univ Technol, Minist Educ, Lab Mat Modificat Laser Ion &amp; Electron Beams, Dalian 116024, Peoples R China.</t>
+        </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B73" s="2" t="inlineStr">
         <is>
           <t>Miao, Naihua</t>
         </is>
@@ -3407,12 +4247,12 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY LETTERS</t>
         </is>
       </c>
       <c r="H73" t="n">
@@ -3420,13 +4260,23 @@
       </c>
       <c r="I73" t="n">
         <v>48</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Miao, NH; Sun, ZM (reprint author), Beihang Univ, Sch Mat Sci &amp; Engn, Beijing 100191, Peoples R China.; Miao, NH; Sun, ZM (reprint author), Beihang Univ, Int Res Inst Multidisciplinary Sci, Ctr Integrated Computat Mat Engn, Beijing 100191, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>ZM (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B74" s="2" t="inlineStr">
         <is>
           <t>Sun, Zhimei</t>
         </is>
@@ -3448,12 +4298,12 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY LETTERS</t>
         </is>
       </c>
       <c r="H74" t="n">
@@ -3461,13 +4311,23 @@
       </c>
       <c r="I74" t="n">
         <v>48</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Miao, NH; Sun, ZM (reprint author), Beihang Univ, Sch Mat Sci &amp; Engn, Beijing 100191, Peoples R China.; Miao, NH; Sun, ZM (reprint author), Beihang Univ, Int Res Inst Multidisciplinary Sci, Ctr Integrated Computat Mat Engn, Beijing 100191, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>ZM (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B75" s="2" t="inlineStr">
         <is>
           <t>Zhang, Z. H.</t>
         </is>
@@ -3489,12 +4349,12 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>JOURNAL OF MATERIALS CHEMISTRY C</t>
         </is>
       </c>
       <c r="H75" t="n">
@@ -3502,13 +4362,23 @@
       </c>
       <c r="I75" t="n">
         <v>68</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Zhang, ZH (reprint author), Changsha Univ Sci &amp; Technol, Hunan Prov Key Lab Flexible Elect Mat Genome Engn, Changsha 410114, Hunan, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Changsha Univ Sci &amp; Technol</t>
+        </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B76" s="2" t="inlineStr">
         <is>
           <t>Liu, Guodong</t>
         </is>
@@ -3530,12 +4400,12 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY C</t>
         </is>
       </c>
       <c r="H76" t="n">
@@ -3543,13 +4413,23 @@
       </c>
       <c r="I76" t="n">
         <v>40</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Liu, GD (reprint author), Hebei Univ Technol, State Key Lab Reliabil &amp; Intelligence Elect Equip, Tianjin 300130, Peoples R China.; Liu, GD (reprint author), Hebei Univ Technol, Sch Mat Sci &amp; Engn, Tianjin 300130, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Hebei Univ Technol</t>
+        </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B77" s="2" t="inlineStr">
         <is>
           <t>Ruan, Shuangchen</t>
         </is>
@@ -3571,12 +4451,12 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H77" t="n">
@@ -3584,13 +4464,23 @@
       </c>
       <c r="I77" t="n">
         <v>222</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Ruan, SC; Zeng, YJ (reprint author), Shenzhen Univ, Coll Phys &amp; Optoelect Engn, Shenzhen 518060, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>YJ (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B78" s="2" t="inlineStr">
         <is>
           <t>Zeng, Yu-Jia</t>
         </is>
@@ -3612,12 +4502,12 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H78" t="n">
@@ -3625,20 +4515,30 @@
       </c>
       <c r="I78" t="n">
         <v>222</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Ruan, SC; Zeng, YJ (reprint author), Shenzhen Univ, Coll Phys &amp; Optoelect Engn, Shenzhen 518060, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>YJ (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Yang, Teng</t>
+      <c r="B79" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Yang</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3653,12 +4553,12 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>CHINESE PHYSICS B</t>
         </is>
       </c>
       <c r="H79" t="n">
@@ -3666,13 +4566,33 @@
       </c>
       <c r="I79" t="n">
         <v>44</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Yang, T (reprint author), Chinese Acad Sci, Inst Met Res, Shenyang Natl Lab Mat Sci, Shenyang 110016, Liaoning, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Chinese Acad Sci</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Wang, Ji-Zhang; Huang, Jian-Qi; Wang, Ya-Ning; Yang, Teng; Zhang, Zhi-Dong</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>Yang, T (reprint author), Chinese Acad Sci, Inst Met Res, Shenyang Natl Lab Mat Sci, Shenyang 110016, Liaoning, Peoples R China.</t>
+        </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="B80" s="2" t="inlineStr">
         <is>
           <t>Kadkhodaei, Mahmoud</t>
         </is>
@@ -3694,12 +4614,12 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>NEW YORK</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>SPRINGER</t>
+          <t>CONTINUUM MECHANICS AND THERMODYNAMICS</t>
         </is>
       </c>
       <c r="H80" t="n">
@@ -3707,13 +4627,23 @@
       </c>
       <c r="I80" t="n">
         <v>63</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Kadkhodaei, M (reprint author), Isfahan Univ Technol, Dept Mech Engn, Esfahan 8415683111, Iran.</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Isfahan Univ Technol</t>
+        </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B81" s="2" t="inlineStr">
         <is>
           <t>Du, Kui</t>
         </is>
@@ -3735,12 +4665,12 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>NANO LETTERS</t>
         </is>
       </c>
       <c r="H81" t="n">
@@ -3748,13 +4678,23 @@
       </c>
       <c r="I81" t="n">
         <v>35</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Du, K (reprint author), Chinese Acad Sci, Shenyang Natl Lab Mat Sci, Inst Met Res, Shenyang 110016, Liaoning, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Chinese Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B82" s="3" t="inlineStr">
         <is>
           <t>Wierzbowska, Malgorzata</t>
         </is>
@@ -3776,12 +4716,12 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>CHAM</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>SPRINGER INTERNATIONAL PUBLISHING AG</t>
+          <t>SN APPLIED SCIENCES</t>
         </is>
       </c>
       <c r="H82" t="n">
@@ -3789,13 +4729,23 @@
       </c>
       <c r="I82" t="n">
         <v>52</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Wierzbowska, M (reprint author), Polish Acad Sci, Inst High Pressure Phys, Sokolowska 29-37, PL-01142 Warsaw, Poland.</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Polish Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B83" s="2" t="inlineStr">
         <is>
           <t>Chen, Yunfei</t>
         </is>
@@ -3817,12 +4767,12 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>NANOSCALE HORIZONS</t>
         </is>
       </c>
       <c r="H83" t="n">
@@ -3830,13 +4780,23 @@
       </c>
       <c r="I83" t="n">
         <v>47</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Chen, YF (reprint author), Southeast Univ, Sch Mech Engn, Nanjing 211189, Jiangsu, Peoples R China.; Wang, JL (reprint author), Southeast Univ, Sch Phys, Nanjing 211189, Jiangsu, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Southeast Univ</t>
+        </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B84" s="2" t="inlineStr">
         <is>
           <t>Wang, Jinlan</t>
         </is>
@@ -3858,12 +4818,12 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>NANOSCALE HORIZONS</t>
         </is>
       </c>
       <c r="H84" t="n">
@@ -3871,13 +4831,23 @@
       </c>
       <c r="I84" t="n">
         <v>47</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Chen, YF (reprint author), Southeast Univ, Sch Mech Engn, Nanjing 211189, Jiangsu, Peoples R China.; Wang, JL (reprint author), Southeast Univ, Sch Phys, Nanjing 211189, Jiangsu, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Southeast Univ</t>
+        </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B85" s="3" t="inlineStr">
         <is>
           <t>Avsar, Ahmet</t>
         </is>
@@ -3899,12 +4869,12 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>LONDON</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>NATURE PUBLISHING GROUP</t>
+          <t>NATURE NANOTECHNOLOGY</t>
         </is>
       </c>
       <c r="H85" t="n">
@@ -3912,13 +4882,23 @@
       </c>
       <c r="I85" t="n">
         <v>40</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Avsar, A; Kis, A (reprint author), Ecole Polytech Fed Lausanne, Elect Engn Inst, Lausanne, Switzerland.; Avsar, A; Kis, A (reprint author), Ecole Polytech Fed Lausanne, Inst Mat Sci &amp; Engn, Lausanne, Switzerland.</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>A (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B86" s="3" t="inlineStr">
         <is>
           <t>Kis, Andras</t>
         </is>
@@ -3940,12 +4920,12 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>LONDON</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>NATURE PUBLISHING GROUP</t>
+          <t>NATURE NANOTECHNOLOGY</t>
         </is>
       </c>
       <c r="H86" t="n">
@@ -3953,13 +4933,23 @@
       </c>
       <c r="I86" t="n">
         <v>40</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Avsar, A; Kis, A (reprint author), Ecole Polytech Fed Lausanne, Elect Engn Inst, Lausanne, Switzerland.; Avsar, A; Kis, A (reprint author), Ecole Polytech Fed Lausanne, Inst Mat Sci &amp; Engn, Lausanne, Switzerland.</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>A (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B87" s="2" t="inlineStr">
         <is>
           <t>Zhang, Mingzhe</t>
         </is>
@@ -3981,12 +4971,12 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>AMSTERDAM</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>ELSEVIER SCIENCE BV</t>
+          <t>APPLIED SURFACE SCIENCE</t>
         </is>
       </c>
       <c r="H87" t="n">
@@ -3994,13 +4984,23 @@
       </c>
       <c r="I87" t="n">
         <v>37</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Zhang, MZ (reprint author), Jilin Univ, State Key Lab Superhard Mat, Changchun 130012, Jilin, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Jilin Univ</t>
+        </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B88" s="3" t="inlineStr">
         <is>
           <t>Tresca, Cesare</t>
         </is>
@@ -4022,12 +5022,12 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>2D MATERIALS</t>
         </is>
       </c>
       <c r="H88" t="n">
@@ -4035,13 +5035,23 @@
       </c>
       <c r="I88" t="n">
         <v>38</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Tresca, C (reprint author), Sorbonne Univ, Inst Nanosci Paris, UMR7588, CNRS, F-75252 Paris, France.</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Sorbonne Univ</t>
+        </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B89" s="3" t="inlineStr">
         <is>
           <t>Calandra, Matteo</t>
         </is>
@@ -4063,12 +5073,12 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>France</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>2D MATERIALS</t>
         </is>
       </c>
       <c r="H89" t="n">
@@ -4076,13 +5086,23 @@
       </c>
       <c r="I89" t="n">
         <v>38</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Tresca, C (reprint author), Sorbonne Univ, Inst Nanosci Paris, UMR7588, CNRS, F-75252 Paris, France.</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sorbonne Univ</t>
+        </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B90" s="2" t="inlineStr">
         <is>
           <t>Lu, Jianchen</t>
         </is>
@@ -4097,19 +5117,19 @@
           <t>Half-metallicity in a honeycomb-kagome-lattice Mg3Si2 monolayer with carrier doping</t>
         </is>
       </c>
-      <c r="E90" s="2" t="inlineStr">
+      <c r="E90" t="inlineStr">
         <is>
           <t>lu.jianchen1989@gmail.com</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>MATERIALS RESEARCH EXPRESS</t>
         </is>
       </c>
       <c r="H90" t="n">
@@ -4117,13 +5137,23 @@
       </c>
       <c r="I90" t="n">
         <v>46</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Lu, JC; Yan, CX; Cai, JM (reprint author), Kunming Univ Sci &amp; Technol, Fac Mat Sci &amp; Engn, Kunming 650093, Yunnan, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>CX; Cai</t>
+        </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="B91" s="2" t="inlineStr">
         <is>
           <t>Yan, Cuixia</t>
         </is>
@@ -4138,19 +5168,19 @@
           <t>Half-metallicity in a honeycomb-kagome-lattice Mg3Si2 monolayer with carrier doping</t>
         </is>
       </c>
-      <c r="E91" s="2" t="inlineStr">
+      <c r="E91" t="inlineStr">
         <is>
           <t>cuixiayan09@gmail.com</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>MATERIALS RESEARCH EXPRESS</t>
         </is>
       </c>
       <c r="H91" t="n">
@@ -4158,13 +5188,23 @@
       </c>
       <c r="I91" t="n">
         <v>46</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Lu, JC; Yan, CX; Cai, JM (reprint author), Kunming Univ Sci &amp; Technol, Fac Mat Sci &amp; Engn, Kunming 650093, Yunnan, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>CX; Cai</t>
+        </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B92" t="inlineStr">
+      <c r="B92" s="2" t="inlineStr">
         <is>
           <t>Cai, Jinming</t>
         </is>
@@ -4186,12 +5226,12 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>MATERIALS RESEARCH EXPRESS</t>
         </is>
       </c>
       <c r="H92" t="n">
@@ -4199,13 +5239,23 @@
       </c>
       <c r="I92" t="n">
         <v>46</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Lu, JC; Yan, CX; Cai, JM (reprint author), Kunming Univ Sci &amp; Technol, Fac Mat Sci &amp; Engn, Kunming 650093, Yunnan, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>CX; Cai</t>
+        </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="B93" s="6" t="inlineStr">
         <is>
           <t>Mendes, J. B. S.</t>
         </is>
@@ -4227,12 +5277,12 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW B</t>
         </is>
       </c>
       <c r="H93" t="n">
@@ -4240,13 +5290,23 @@
       </c>
       <c r="I93" t="n">
         <v>85</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Mendes, JBS (reprint author), Univ Fed Vicosa, Dept Fis, BR-36570900 Vicosa, MG, Brazil.</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Univ Fed Vicosa</t>
+        </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="B94" s="7" t="inlineStr">
         <is>
           <t>Cheng, Zhenxiang</t>
         </is>
@@ -4268,12 +5328,12 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -4281,13 +5341,23 @@
       </c>
       <c r="I94" t="n">
         <v>35</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Cheng, ZX; Wang, YX (reprint author), Henan Univ, Sch Phys &amp; Elect, Inst Computat Mat Sci, Kaifeng 475004, Peoples R China.; Cheng, ZX (reprint author), Univ Wollongong, Australian Inst Innovat Mat, Inst Superconducting &amp; Elect Mat, Wollongong, NSW 2500, Australia.</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>YX (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="B95" s="7" t="inlineStr">
         <is>
           <t>Wang, Yuanxu</t>
         </is>
@@ -4309,12 +5379,12 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H95" t="n">
@@ -4322,20 +5392,30 @@
       </c>
       <c r="I95" t="n">
         <v>35</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Cheng, ZX; Wang, YX (reprint author), Henan Univ, Sch Phys &amp; Elect, Inst Computat Mat Sci, Kaifeng 475004, Peoples R China.; Cheng, ZX (reprint author), Univ Wollongong, Australian Inst Innovat Mat, Inst Superconducting &amp; Elect Mat, Wollongong, NSW 2500, Australia.</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>YX (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Xiao, Haibo</t>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Xiao</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -4350,12 +5430,12 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H96" t="n">
@@ -4363,13 +5443,33 @@
       </c>
       <c r="I96" t="n">
         <v>66</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>Xiao, HB; Yang, CP (reprint author), Hubei Univ, Fac Phys &amp; Elect Sci, Hubei Key Lab Ferro &amp; Piezoelect Mat &amp; Devices, Wuhan 430062, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>CP (reprint author)</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Xiao, Haibo; Wang, Xiaonan; Wang, Ruilong; Xu, Lingfang; Liang, Shiheng; Yang, Changping</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>Xiao, HB; Yang, CP (reprint author), Hubei Univ, Fac Phys &amp; Elect Sci, Hubei Key Lab Ferro &amp; Piezoelect Mat &amp; Devices, Wuhan 430062, Peoples R China.</t>
+        </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B97" t="inlineStr">
+      <c r="B97" s="2" t="inlineStr">
         <is>
           <t>Yang, Changping</t>
         </is>
@@ -4391,12 +5491,12 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>PHYSICAL CHEMISTRY CHEMICAL PHYSICS</t>
         </is>
       </c>
       <c r="H97" t="n">
@@ -4404,13 +5504,23 @@
       </c>
       <c r="I97" t="n">
         <v>66</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>Xiao, HB; Yang, CP (reprint author), Hubei Univ, Fac Phys &amp; Elect Sci, Hubei Key Lab Ferro &amp; Piezoelect Mat &amp; Devices, Wuhan 430062, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>CP (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98" t="inlineStr">
+      <c r="B98" s="5" t="inlineStr">
         <is>
           <t>Hwang, Chanyong</t>
         </is>
@@ -4432,12 +5542,12 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>Korea</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>NANOTECHNOLOGY</t>
         </is>
       </c>
       <c r="H98" t="n">
@@ -4445,13 +5555,23 @@
       </c>
       <c r="I98" t="n">
         <v>42</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>Hwang, C (reprint author), Korea Res Inst Stand &amp; Sci, Quantum Technol Inst, Daejeon 34113, South Korea.</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>Korea Res Inst Stand &amp; Sci</t>
+        </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B99" s="3" t="inlineStr">
         <is>
           <t>Maletinsky, P.</t>
         </is>
@@ -4473,12 +5593,12 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>AMER ASSOC ADVANCEMENT SCIENCE</t>
+          <t>SCIENCE</t>
         </is>
       </c>
       <c r="H99" t="n">
@@ -4486,13 +5606,23 @@
       </c>
       <c r="I99" t="n">
         <v>39</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>Maletinsky, P (reprint author), Univ Basel, Dept Phys, Klingelbergstr 82, CH-4056 Basel, Switzerland.</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>Univ Basel</t>
+        </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B100" t="inlineStr">
+      <c r="B100" s="2" t="inlineStr">
         <is>
           <t>Zhang, Min</t>
         </is>
@@ -4514,12 +5644,12 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>JOURNAL OF MATERIALS CHEMISTRY C</t>
         </is>
       </c>
       <c r="H100" t="n">
@@ -4527,20 +5657,30 @@
       </c>
       <c r="I100" t="n">
         <v>81</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>Zhang, M (reprint author), Northeast Normal Univ, Fac Chem, Inst Funct Mat Chem, Changchun 130024, Jilin, Peoples R China.; Zhang, M (reprint author), Northeast Normal Univ, Natl &amp; Local United Engn Lab Power Battery, Changchun 130024, Jilin, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, CAS Ctr Excellence Nanosci, Sch Chem &amp; Mat Sci, CAS Key Lab Mat Energy Convers, Hefei 230026, Anhui, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Li, YF (reprint author), Nanjing Normal Univ, Sch Chem &amp; Mat Sci, Jiangsu Key Lab New Power Batteries, Jiangsu Collaborat Innovat Ctr Biomed Funct Mat, Nanjing 210023, Jiangsu, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Northeast Normal Univ</t>
+        </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Wu, Xiaojun</t>
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Wu</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -4555,12 +5695,12 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>JOURNAL OF MATERIALS CHEMISTRY C</t>
         </is>
       </c>
       <c r="H101" t="n">
@@ -4568,13 +5708,33 @@
       </c>
       <c r="I101" t="n">
         <v>81</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>Zhang, M (reprint author), Northeast Normal Univ, Fac Chem, Inst Funct Mat Chem, Changchun 130024, Jilin, Peoples R China.; Zhang, M (reprint author), Northeast Normal Univ, Natl &amp; Local United Engn Lab Power Battery, Changchun 130024, Jilin, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, CAS Ctr Excellence Nanosci, Sch Chem &amp; Mat Sci, CAS Key Lab Mat Energy Convers, Hefei 230026, Anhui, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Li, YF (reprint author), Nanjing Normal Univ, Sch Chem &amp; Mat Sci, Jiangsu Key Lab New Power Batteries, Jiangsu Collaborat Innovat Ctr Biomed Funct Mat, Nanjing 210023, Jiangsu, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Northeast Normal Univ</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>Zhu, Changyan; Lv, Haifeng; Qu, Xin; Zhang, Min; Wang, Jianyun; Wen, Shizheng; Li, Quan; Geng, Yun; Su, Zhongmin; Wu, Xiaojun; Li, Yafei; Ma, Yanming</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>Zhang, M (reprint author), Northeast Normal Univ, Fac Chem, Inst Funct Mat Chem, Changchun 130024, Jilin, Peoples R China.; Zhang, M (reprint author), Northeast Normal Univ, Natl &amp; Local United Engn Lab Power Battery, Changchun 130024, Jilin, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, CAS Ctr Excellence Nanosci, Sch Chem &amp; Mat Sci, CAS Key Lab Mat Energy Convers, Hefei 230026, Anhui, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Li, YF (reprint author), Nanjing Normal Univ, Sch Chem &amp; Mat Sci, Jiangsu Key Lab New Power Batteries, Jiangsu Collaborat Innovat Ctr Biomed Funct Mat, Nanjing 210023, Jiangsu, Peoples R China.</t>
+        </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B102" t="inlineStr">
+      <c r="B102" s="2" t="inlineStr">
         <is>
           <t>Li, Yafei</t>
         </is>
@@ -4596,12 +5756,12 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>CAMBRIDGE</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>ROYAL SOC CHEMISTRY</t>
+          <t>JOURNAL OF MATERIALS CHEMISTRY C</t>
         </is>
       </c>
       <c r="H102" t="n">
@@ -4609,13 +5769,23 @@
       </c>
       <c r="I102" t="n">
         <v>81</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>Zhang, M (reprint author), Northeast Normal Univ, Fac Chem, Inst Funct Mat Chem, Changchun 130024, Jilin, Peoples R China.; Zhang, M (reprint author), Northeast Normal Univ, Natl &amp; Local United Engn Lab Power Battery, Changchun 130024, Jilin, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, CAS Ctr Excellence Nanosci, Sch Chem &amp; Mat Sci, CAS Key Lab Mat Energy Convers, Hefei 230026, Anhui, Peoples R China.; Wu, XJ (reprint author), Univ Sci &amp; Technol China, Hefei Natl Lab Phys Sci Microscale, Hefei 230026, Anhui, Peoples R China.; Li, YF (reprint author), Nanjing Normal Univ, Sch Chem &amp; Mat Sci, Jiangsu Key Lab New Power Batteries, Jiangsu Collaborat Innovat Ctr Biomed Funct Mat, Nanjing 210023, Jiangsu, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Northeast Normal Univ</t>
+        </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B103" t="inlineStr">
+      <c r="B103" s="2" t="inlineStr">
         <is>
           <t>Zhang, Jun</t>
         </is>
@@ -4637,12 +5807,12 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>WASHINGTON</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>AMER CHEMICAL SOC</t>
+          <t>JOURNAL OF PHYSICAL CHEMISTRY LETTERS</t>
         </is>
       </c>
       <c r="H103" t="n">
@@ -4650,13 +5820,23 @@
       </c>
       <c r="I103" t="n">
         <v>43</v>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>Zhang, J (reprint author), Chinese Acad Sci, Inst Semicond, State Key Lab Superlattices &amp; Microstruct, Beijing 100083, Peoples R China.; Zhang, J (reprint author), Univ Chinese Acad Sci, Ctr Mat Sci &amp; Optoelect Engn, Beijing 100049, Peoples R China.; Zhang, J (reprint author), Univ Chinese Acad Sci, CAS Ctr Excellence Topol Quantum Computat, Beijing 101408, Peoples R China.; Zhang, J (reprint author), Beijing Acad Quantum Informat Sci, Beijing 100193, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Chinese Acad Sci</t>
+        </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B104" t="inlineStr">
+      <c r="B104" s="5" t="inlineStr">
         <is>
           <t>Choi, Jun-Hyung</t>
         </is>
@@ -4678,12 +5858,12 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>COLLEGE PK</t>
+          <t>Korea</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>AMER PHYSICAL SOC</t>
+          <t>PHYSICAL REVIEW B</t>
         </is>
       </c>
       <c r="H104" t="n">
@@ -4691,20 +5871,30 @@
       </c>
       <c r="I104" t="n">
         <v>42</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>Choi, JH (reprint author), Hanyang Univ, HYU HPSTAR CIS High Pressure Res Ctr, Res Inst Nat Sci, Dept Phys, Seoul 133791, South Korea.</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>Hanyang Univ</t>
+        </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Torelli, Piero</t>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>de Jong, Michel P.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Torelli</t>
+          <t>de Jong</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -4719,12 +5909,12 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H105" t="n">
@@ -4732,13 +5922,23 @@
       </c>
       <c r="I105" t="n">
         <v>51</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, Ctr Adv 2D Mat CA2DM, 6 Sci Dr 2, Singapore 117546, Singapore.; Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, GRC, 6 Sci Dr 2, Singapore 117546, Singapore.; Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, Dept Phys, 2 Sci Dr 3, Singapore 117542, Singapore.; de Jong, MP (reprint author), Univ Twente, NanoElect Grp, MESA Inst Nanotechnol, POB 217, NL-7500 AE Enschede, Netherlands.</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>ATS (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B106" t="inlineStr">
+      <c r="B106" s="3" t="inlineStr">
         <is>
           <t>Neto, Antonio H. Castro</t>
         </is>
@@ -4760,12 +5960,12 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H106" t="n">
@@ -4773,13 +5973,23 @@
       </c>
       <c r="I106" t="n">
         <v>51</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, Ctr Adv 2D Mat CA2DM, 6 Sci Dr 2, Singapore 117546, Singapore.; Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, GRC, 6 Sci Dr 2, Singapore 117546, Singapore.; Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, Dept Phys, 2 Sci Dr 3, Singapore 117542, Singapore.; de Jong, MP (reprint author), Univ Twente, NanoElect Grp, MESA Inst Nanotechnol, POB 217, NL-7500 AE Enschede, Netherlands.</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>ATS (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="B107" t="inlineStr">
+      <c r="B107" s="3" t="inlineStr">
         <is>
           <t>Wee, Andrew Thye Shen</t>
         </is>
@@ -4801,12 +6011,12 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>WEINHEIM</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>WILEY-V C H VERLAG GMBH</t>
+          <t>ADVANCED MATERIALS</t>
         </is>
       </c>
       <c r="H107" t="n">
@@ -4814,13 +6024,23 @@
       </c>
       <c r="I107" t="n">
         <v>51</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, Ctr Adv 2D Mat CA2DM, 6 Sci Dr 2, Singapore 117546, Singapore.; Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, GRC, 6 Sci Dr 2, Singapore 117546, Singapore.; Neto, AHC; Wee, ATS (reprint author), Natl Univ Singapore, Dept Phys, 2 Sci Dr 3, Singapore 117542, Singapore.; de Jong, MP (reprint author), Univ Twente, NanoElect Grp, MESA Inst Nanotechnol, POB 217, NL-7500 AE Enschede, Netherlands.</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>ATS (reprint author)</t>
+        </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="B108" t="inlineStr">
+      <c r="B108" s="2" t="inlineStr">
         <is>
           <t>Zhang, Lei</t>
         </is>
@@ -4842,12 +6062,12 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>JOURNAL OF SEMICONDUCTORS</t>
         </is>
       </c>
       <c r="H108" t="n">
@@ -4855,13 +6075,23 @@
       </c>
       <c r="I108" t="n">
         <v>100</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>Zhang, L (reprint author), Xi An Jiao Tong Univ, Sch Sci, MOE Key Lab Nonequilibrium Synth &amp; Modulat Conden, Xian 710049, Shaanxi, Peoples R China.; Liu, K (reprint author), Tsinghua Univ, Sch Mat Sci &amp; Engn, State Key Lab New Ceram &amp; Fine Proc, Beijing 100084, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Xi An Jiao Tong Univ</t>
+        </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="B109" t="inlineStr">
+      <c r="B109" s="2" t="inlineStr">
         <is>
           <t>Liu, Kai</t>
         </is>
@@ -4883,12 +6113,12 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>BRISTOL</t>
+          <t>China</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>IOP PUBLISHING LTD</t>
+          <t>JOURNAL OF SEMICONDUCTORS</t>
         </is>
       </c>
       <c r="H109" t="n">
@@ -4896,6 +6126,16 @@
       </c>
       <c r="I109" t="n">
         <v>100</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>Zhang, L (reprint author), Xi An Jiao Tong Univ, Sch Sci, MOE Key Lab Nonequilibrium Synth &amp; Modulat Conden, Xian 710049, Shaanxi, Peoples R China.; Liu, K (reprint author), Tsinghua Univ, Sch Mat Sci &amp; Engn, State Key Lab New Ceram &amp; Fine Proc, Beijing 100084, Peoples R China.</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Xi An Jiao Tong Univ</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>